<commit_message>
All changes from incomplete unit testing and SMB.
</commit_message>
<xml_diff>
--- a/mihc/tumor_screening.xlsx
+++ b/mihc/tumor_screening.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/becca/Dropbox/Mac (3)/Documents/Postdoc/Code/breast_cancer/Model/mihc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26621D19-B15C-3142-B8E5-FEAE288231C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4931A9AB-6AEA-374A-90E2-5403D0A7E94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-51200" yWindow="2040" windowWidth="51200" windowHeight="28300" xr2:uid="{86DCD173-A932-4C44-9AFA-FAC3A2C1AD5B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="69">
   <si>
     <t>'121223 P9msP61-2 #01 NT2.5 LM Lungs 10d-1_met_1.csv_down_sample.csv'</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>SMB</t>
+  </si>
+  <si>
+    <t>SMB?</t>
   </si>
 </sst>
 </file>
@@ -635,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064637B2-6FDF-D740-ABDE-F5E167C79555}">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="163" workbookViewId="0">
-      <selection activeCell="M59" sqref="M59"/>
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -862,9 +865,6 @@
         <f>SUM($I$2:$I11)</f>
         <v>6</v>
       </c>
-      <c r="M11" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -960,7 +960,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -983,7 +983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -999,7 +999,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -1037,8 +1037,11 @@
         <f>SUM($I$2:$I20)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -1107,7 +1110,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
@@ -1130,7 +1133,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -1153,7 +1156,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
@@ -1176,7 +1179,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
@@ -1199,7 +1202,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
@@ -1222,7 +1225,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
@@ -1245,7 +1248,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
@@ -1268,7 +1271,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
@@ -1291,7 +1294,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
@@ -1314,7 +1317,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
@@ -1337,7 +1340,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>32</v>
       </c>
@@ -1360,7 +1363,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>33</v>
       </c>
@@ -1383,7 +1386,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>34</v>
       </c>
@@ -1406,7 +1409,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>35</v>
       </c>
@@ -1429,7 +1432,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
@@ -1452,7 +1455,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>37</v>
       </c>
@@ -1475,7 +1478,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>38</v>
       </c>
@@ -1498,7 +1501,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>39</v>
       </c>
@@ -1521,7 +1524,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>40</v>
       </c>
@@ -1544,7 +1547,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1560,7 +1563,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1576,7 +1579,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>43</v>
       </c>
@@ -1599,7 +1602,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>44</v>
       </c>
@@ -1621,11 +1624,8 @@
         <f>SUM($I$2:$I46)</f>
         <v>34</v>
       </c>
-      <c r="M46" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>45</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>46</v>
       </c>
@@ -1739,9 +1739,6 @@
         <f>SUM($I$2:$I51)</f>
         <v>39</v>
       </c>
-      <c r="M51" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
@@ -1804,9 +1801,6 @@
         <f>SUM($I$2:$I54)</f>
         <v>41</v>
       </c>
-      <c r="M54" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
@@ -1954,6 +1948,9 @@
         <f>SUM($I$2:$I61)</f>
         <v>46</v>
       </c>
+      <c r="M61" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>